<commit_message>
Get statistics of STSJC3
</commit_message>
<xml_diff>
--- a/statistics.xlsx
+++ b/statistics.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="听说教程3" sheetId="1" r:id="rId1"/>
+    <sheet name="视听说教程3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="160">
   <si>
     <t>Listening</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -570,6 +571,86 @@
   </si>
   <si>
     <t>407</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ouside view</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Listening in</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Activity 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Activity 2</t>
+  </si>
+  <si>
+    <t>Activity 3</t>
+  </si>
+  <si>
+    <t>Activity 4</t>
+  </si>
+  <si>
+    <t>Passage 1: Activity 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passage 1: Activity 2</t>
+  </si>
+  <si>
+    <t>Passage 1: Activity 3</t>
+  </si>
+  <si>
+    <t>Passage 2: Activity 1</t>
+  </si>
+  <si>
+    <t>Passage 2: Activity 2</t>
+  </si>
+  <si>
+    <t>Passage 2: Activity 3</t>
+  </si>
+  <si>
+    <t>Target: 10.13.54.81/book/book41/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj31drag.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj34mc.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj31checkboxTable.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj34drag.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj44mc.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj41blank.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj42drag.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj42drag.php/dj44dragOne.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dj45checkboxTable.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -702,7 +783,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -775,6 +856,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,6 +881,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1081,9 +1168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N32" sqref="N32"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1132,46 +1219,46 @@
       <c r="H1" s="3"/>
       <c r="I1" s="4"/>
       <c r="J1" s="22"/>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="26" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="24" t="s">
+      <c r="N1" s="28"/>
+      <c r="O1" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="24" t="s">
+      <c r="P1" s="26"/>
+      <c r="Q1" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="24" t="s">
+      <c r="R1" s="26"/>
+      <c r="S1" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="25"/>
-      <c r="U1" s="24" t="s">
+      <c r="T1" s="26"/>
+      <c r="U1" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="24" t="s">
+      <c r="V1" s="26"/>
+      <c r="W1" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="24" t="s">
+      <c r="X1" s="26"/>
+      <c r="Y1" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="24" t="s">
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="24" t="s">
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="AD1" s="25"/>
+      <c r="AD1" s="26"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -1260,10 +1347,10 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1332,8 +1419,8 @@
       <c r="AD3" s="7"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="31"/>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1400,8 +1487,8 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
@@ -1468,8 +1555,8 @@
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="30"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
@@ -1556,8 +1643,8 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="30" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
@@ -1592,8 +1679,8 @@
       <c r="AD7" s="10"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="30"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
@@ -1626,8 +1713,8 @@
       <c r="AD8" s="10"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="30"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="5" t="s">
         <v>33</v>
       </c>
@@ -1714,7 +1801,7 @@
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="5" t="s">
         <v>2</v>
       </c>
@@ -1750,8 +1837,8 @@
       <c r="AD10" s="10"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="31" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1840,8 +1927,8 @@
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" s="28"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1928,8 +2015,8 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" s="28"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
@@ -2016,8 +2103,8 @@
       </c>
     </row>
     <row r="14" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="11" t="s">
         <v>14</v>
       </c>
@@ -2142,4 +2229,141 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="33"/>
+      <c r="B7" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B12"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>